<commit_message>
Exported PNG images of results
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Advanced Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF40374-6DAB-498E-AB7B-F0DB6ADA27B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA71558-94A0-4AA5-94A6-B780130AA281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9756" yWindow="3780" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{5FE45F75-0CBC-4D78-8844-891CA4419193}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{5FE45F75-0CBC-4D78-8844-891CA4419193}"/>
   </bookViews>
   <sheets>
     <sheet name="10x10x10" sheetId="1" r:id="rId1"/>
@@ -234,7 +234,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Multiple values by 'Time'</a:t>
+              <a:t>Results of the 10x10x10</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1687,9 +1687,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Multiple values by 'Time'</a:t>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Results of the 15x15x15</a:t>
             </a:r>
+            <a:endParaRPr lang="en-NL">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3141,9 +3146,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Multiple values by 'Time'</a:t>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Results of the 20x20x20</a:t>
             </a:r>
+            <a:endParaRPr lang="en-NL">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -6654,7 +6664,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G26"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7877,7 +7887,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>